<commit_message>
Added tests, work on traversal
</commit_message>
<xml_diff>
--- a/src/main/resources/Basic strategy.xlsx
+++ b/src/main/resources/Basic strategy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="22995" windowHeight="13800"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="22995" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Strategy" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="31">
   <si>
     <t>S</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>(A, A)</t>
+  </si>
+  <si>
+    <t>(T, T)</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -453,30 +456,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -919,6 +898,30 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -967,43 +970,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="52" name="Table52" displayName="Table52" ref="B2:M36" tableType="xml" totalsRowShown="0" dataDxfId="0" connectionId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="52" name="Table52" displayName="Table52" ref="B2:M36" tableType="xml" totalsRowShown="0" dataDxfId="12" connectionId="13">
   <autoFilter ref="B2:M36"/>
   <tableColumns count="12">
-    <tableColumn id="1" uniqueName="playerHand" name="playerHand" dataDxfId="12">
+    <tableColumn id="1" uniqueName="playerHand" name="playerHand" dataDxfId="11">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/playerHand" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="totalType" name="totalType" dataDxfId="11">
+    <tableColumn id="2" uniqueName="totalType" name="totalType" dataDxfId="10">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/totalType" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="action_2" name="action_2" dataDxfId="10">
+    <tableColumn id="3" uniqueName="action_2" name="action_2" dataDxfId="9">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/action_2" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="action_3" name="action_3" dataDxfId="9">
+    <tableColumn id="4" uniqueName="action_3" name="action_3" dataDxfId="8">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/action_3" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="action_4" name="action_4" dataDxfId="8">
+    <tableColumn id="5" uniqueName="action_4" name="action_4" dataDxfId="7">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/action_4" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="action_5" name="action_5" dataDxfId="7">
+    <tableColumn id="6" uniqueName="action_5" name="action_5" dataDxfId="6">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/action_5" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="action_6" name="action_6" dataDxfId="6">
+    <tableColumn id="7" uniqueName="action_6" name="action_6" dataDxfId="5">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/action_6" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="action_7" name="action_7" dataDxfId="5">
+    <tableColumn id="8" uniqueName="action_7" name="action_7" dataDxfId="4">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/action_7" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="action_8" name="action_8" dataDxfId="4">
+    <tableColumn id="9" uniqueName="action_8" name="action_8" dataDxfId="3">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/action_8" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="action_9" name="action_9" dataDxfId="3">
+    <tableColumn id="10" uniqueName="action_9" name="action_9" dataDxfId="2">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/action_9" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="action_T" name="action_T" dataDxfId="2">
+    <tableColumn id="11" uniqueName="action_T" name="action_T" dataDxfId="1">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/action_T" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="action_A" name="action_A" dataDxfId="1">
+    <tableColumn id="12" uniqueName="action_A" name="action_A" dataDxfId="0">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/action_A" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -1301,7 +1304,7 @@
   <dimension ref="A2:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,34 +1363,34 @@
       <c r="C3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="16" t="s">
+      <c r="D3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="15" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1989,34 +1992,34 @@
       <c r="C19" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="M19" s="16" t="s">
+      <c r="D19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="15" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2288,75 +2291,75 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="14">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K27" s="15" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L27" s="15" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M27" s="15" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>0</v>
+      <c r="D28" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>0</v>
+      <c r="J28" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>0</v>
@@ -2367,7 +2370,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>14</v>
@@ -2387,8 +2390,8 @@
       <c r="H29" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I29" s="4" t="s">
-        <v>0</v>
+      <c r="I29" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>5</v>
@@ -2396,16 +2399,16 @@
       <c r="K29" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>0</v>
+      <c r="L29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>14</v>
@@ -2428,22 +2431,22 @@
       <c r="I30" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M30" s="8" t="s">
-        <v>5</v>
+      <c r="J30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>14</v>
@@ -2463,8 +2466,8 @@
       <c r="H31" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>5</v>
+      <c r="I31" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>1</v>
@@ -2481,34 +2484,34 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K32" s="5" t="s">
-        <v>1</v>
+      <c r="D32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="L32" s="5" t="s">
         <v>1</v>
@@ -2517,36 +2520,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K33" s="7" t="s">
-        <v>3</v>
+      <c r="D33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="L33" s="5" t="s">
         <v>1</v>
@@ -2555,21 +2558,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>1</v>
+      <c r="D34" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>5</v>
@@ -2577,8 +2580,8 @@
       <c r="H34" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I34" s="5" t="s">
-        <v>1</v>
+      <c r="I34" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>1</v>
@@ -2593,45 +2596,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="3">
-        <v>3</v>
-      </c>
-      <c r="C35" s="3" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D35" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
       <c r="B36" s="3">
         <v>2</v>
       </c>
@@ -2656,17 +2662,17 @@
       <c r="I36" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J36" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>1</v>
+      <c r="J36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M36" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
many more tests and fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/Basic strategy.xlsx
+++ b/src/main/resources/Basic strategy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="22995" windowHeight="13740"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="22995" windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Strategy" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="32">
   <si>
     <t>S</t>
   </si>
@@ -224,12 +224,15 @@
   <si>
     <t>(T, T)</t>
   </si>
+  <si>
+    <t>&lt;- Occurs when multiple split aces not allowed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +261,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -378,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -427,6 +437,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -970,8 +986,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="52" name="Table52" displayName="Table52" ref="B2:M36" tableType="xml" totalsRowShown="0" dataDxfId="12" connectionId="13">
-  <autoFilter ref="B2:M36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="52" name="Table52" displayName="Table52" ref="B2:M37" tableType="xml" totalsRowShown="0" dataDxfId="12" connectionId="13">
+  <autoFilter ref="B2:M37"/>
   <tableColumns count="12">
     <tableColumn id="1" uniqueName="playerHand" name="playerHand" dataDxfId="11">
       <xmlColumnPr mapId="13" xpath="/Strategy/Hand/playerHand" xmlDataType="string"/>
@@ -1301,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O36"/>
+  <dimension ref="A2:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,7 +1925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>6</v>
       </c>
@@ -1947,7 +1963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="9">
         <v>5</v>
       </c>
@@ -1985,7 +2001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
         <v>20</v>
       </c>
@@ -2023,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>19</v>
       </c>
@@ -2061,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>18</v>
       </c>
@@ -2099,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>17</v>
       </c>
@@ -2137,7 +2153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>16</v>
       </c>
@@ -2175,7 +2191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>15</v>
       </c>
@@ -2213,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>14</v>
       </c>
@@ -2251,7 +2267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="9">
         <v>13</v>
       </c>
@@ -2289,88 +2305,91 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="17">
+        <v>12</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="O27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B28" s="14">
         <v>20</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C28" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="K27" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="L27" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="M27" s="15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="3">
+      <c r="D28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M28" s="15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
         <v>18</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="3">
-        <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>14</v>
@@ -2390,8 +2409,8 @@
       <c r="H29" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>5</v>
+      <c r="I29" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>5</v>
@@ -2399,16 +2418,16 @@
       <c r="K29" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M29" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>14</v>
@@ -2431,22 +2450,22 @@
       <c r="I30" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>14</v>
@@ -2466,8 +2485,8 @@
       <c r="H31" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I31" s="5" t="s">
-        <v>1</v>
+      <c r="I31" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>1</v>
@@ -2482,36 +2501,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>3</v>
+      <c r="D32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="L32" s="5" t="s">
         <v>1</v>
@@ -2522,34 +2541,34 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>1</v>
+      <c r="D33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="L33" s="5" t="s">
         <v>1</v>
@@ -2560,19 +2579,19 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>5</v>
+      <c r="D34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>5</v>
@@ -2580,8 +2599,8 @@
       <c r="H34" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I34" s="8" t="s">
-        <v>5</v>
+      <c r="I34" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>1</v>
@@ -2597,81 +2616,119 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="1">
+      <c r="B35" s="3">
+        <v>6</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
         <v>4</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="I35" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="L35" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="M35" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D36" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B37" s="3">
         <v>2</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M36" s="8" t="s">
+      <c r="D37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M37" s="8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>